<commit_message>
Added compatibility with Time domain data
</commit_message>
<xml_diff>
--- a/spreadsheets/attributes_v1.0.xlsx
+++ b/spreadsheets/attributes_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256563FC-EF2B-F540-B09D-3954815DFC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A82F60-A1A5-5649-9A6A-0270FB256DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t>v 0.1</t>
   </si>
@@ -313,13 +313,19 @@
   </si>
   <si>
     <t>MEASURE.Sampling_Matrix_Size_(Nx,Ny,Nz)_()</t>
+  </si>
+  <si>
+    <t>SPECTROMETER.VIPA_FSR_(GHz)</t>
+  </si>
+  <si>
+    <t>The Free Spectral Range of the VIPA used in 1-VIPA spectrometers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,6 +343,18 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -360,10 +378,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,20 +718,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FCBC02-5AB3-D14D-8C37-C0FDD1D4F1E1}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="41.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -725,12 +745,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -741,7 +761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>72</v>
       </c>
@@ -755,7 +775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>90</v>
       </c>
@@ -766,7 +786,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -777,7 +797,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -788,7 +808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -799,7 +819,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -810,7 +830,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -821,12 +841,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -837,7 +857,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -851,7 +871,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -862,7 +882,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -873,7 +893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -884,7 +904,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -898,7 +918,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -909,7 +929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -920,7 +940,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -934,7 +954,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -948,7 +968,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -962,7 +982,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>64</v>
       </c>
@@ -973,7 +993,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -987,7 +1007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1001,7 +1021,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -1015,7 +1035,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1029,7 +1049,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>81</v>
       </c>
@@ -1043,7 +1063,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>68</v>
       </c>
@@ -1054,7 +1074,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -1068,7 +1088,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>83</v>
       </c>
@@ -1082,134 +1102,149 @@
         <v>150</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="34" spans="1:5">
+      <c r="A34" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>84</v>
-      </c>
-      <c r="C34" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>85</v>
       </c>
       <c r="C35" t="s">
         <v>74</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
         <v>74</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E36" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
         <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E37" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
         <v>74</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E38" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
         <v>74</v>
       </c>
       <c r="D39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E40" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
         <v>69</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>73</v>
       </c>
-      <c r="C42" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="C43" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" t="s">
         <v>48</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E43" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
         <v>70</v>
       </c>
-      <c r="C43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
         <v>71</v>
       </c>
-      <c r="C44" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1227,13 +1262,13 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1282,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1261,7 +1296,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Added capabilities to analyze VIPA spectra and created environment to develop new treatment and algorithms
</commit_message>
<xml_diff>
--- a/spreadsheets/attributes_v1.0.xlsx
+++ b/spreadsheets/attributes_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A82F60-A1A5-5649-9A6A-0270FB256DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B52E4F-FFB5-EB4A-AD13-B6F8A4DE2F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
   </bookViews>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FCBC02-5AB3-D14D-8C37-C0FDD1D4F1E1}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added Data validation to the spreadsheet
</commit_message>
<xml_diff>
--- a/spreadsheets/attributes_v1.0.xlsx
+++ b/spreadsheets/attributes_v1.0.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrebouvet/Documents/Code/HDF5_BLS/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B52E4F-FFB5-EB4A-AD13-B6F8A4DE2F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332A09C0-8B2D-254E-9FA3-35D11A108492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" xr2:uid="{43FFD853-F6ED-2B4F-BBE4-F59CF9D7DE1B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Attributes of a measure" sheetId="1" r:id="rId1"/>
-    <sheet name="Attributes of an element" sheetId="2" r:id="rId2"/>
+    <sheet name="Attributes" sheetId="1" r:id="rId1"/>
+    <sheet name="Possible values" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
-  <si>
-    <t>v 0.1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="98">
   <si>
     <t>MEASURE</t>
   </si>
@@ -51,12 +48,6 @@
     <t>FILEPROP</t>
   </si>
   <si>
-    <t>Filepath</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -192,12 +183,6 @@
     <t>Global name of the h5 file</t>
   </si>
   <si>
-    <t>The global filepath to the original file</t>
-  </si>
-  <si>
-    <t>\Users\documents\spectra\raw_spectrum.dat</t>
-  </si>
-  <si>
     <t>MEASURE.Sample</t>
   </si>
   <si>
@@ -319,6 +304,33 @@
   </si>
   <si>
     <t>The Free Spectral Range of the VIPA used in 1-VIPA spectrometers</t>
+  </si>
+  <si>
+    <t>VIPA</t>
+  </si>
+  <si>
+    <t>TFP</t>
+  </si>
+  <si>
+    <t>Time-Domain</t>
+  </si>
+  <si>
+    <t>Stimulated</t>
+  </si>
+  <si>
+    <t>EMCCD</t>
+  </si>
+  <si>
+    <t>sCMOS</t>
+  </si>
+  <si>
+    <t>CCD</t>
+  </si>
+  <si>
+    <t>uss-BM</t>
+  </si>
+  <si>
+    <t>ar-BM</t>
   </si>
 </sst>
 </file>
@@ -720,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FCBC02-5AB3-D14D-8C37-C0FDD1D4F1E1}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -733,54 +745,54 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1">
         <v>0.1</v>
@@ -788,10 +800,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -799,84 +811,84 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E16" s="1">
         <v>532</v>
@@ -884,10 +896,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -895,10 +907,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1">
         <v>0.45</v>
@@ -906,63 +918,63 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E23" s="1">
         <v>0.2</v>
@@ -970,13 +982,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E24" s="1">
         <v>15</v>
@@ -984,38 +996,38 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E27" s="1">
         <v>700</v>
@@ -1023,41 +1035,41 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E30" s="1">
         <v>20</v>
@@ -1065,24 +1077,24 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E32" s="1">
         <v>180</v>
@@ -1090,13 +1102,13 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E33" s="1">
         <v>150</v>
@@ -1104,14 +1116,14 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E34" s="1">
         <v>30</v>
@@ -1119,13 +1131,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D35" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1">
         <v>0.5</v>
@@ -1133,13 +1145,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E36" s="1">
         <v>5</v>
@@ -1147,13 +1159,13 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E37" s="1">
         <v>0.5</v>
@@ -1161,13 +1173,13 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E38" s="1">
         <v>5</v>
@@ -1175,13 +1187,13 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E39" s="1">
         <v>0.5</v>
@@ -1189,13 +1201,13 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E40" s="1">
         <v>50</v>
@@ -1203,21 +1215,21 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B43" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D43" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E43" s="1">
         <v>0.1</v>
@@ -1225,80 +1237,105 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D44" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6CBD64FF-5A74-F54D-A40B-231834318C75}">
+          <x14:formula1>
+            <xm:f>'Possible values'!$B$1:$Z$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>B14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CDC4D4F6-FEDB-0E49-89B8-ED175B3ED998}">
+          <x14:formula1>
+            <xm:f>'Possible values'!$B$2:$Z$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>B20</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10FF49C8-5C81-9E49-9207-DCFD249EB382}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB7322B-3190-9C48-9722-E654FF848AF3}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
+        <v>90</v>
+      </c>
+      <c r="E1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>